<commit_message>
Add backup equipment row to Excel template, shift Documentation section down
Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/templates/rfi_template.xlsx
+++ b/templates/rfi_template.xlsx
@@ -455,7 +455,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C105"/>
+  <dimension ref="A1:C106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,8 +474,6 @@
           <t>Onboarding RFI — Bellwether Technology</t>
         </is>
       </c>
-      <c r="B1" s="2" t="n"/>
-      <c r="C1" s="2" t="n"/>
     </row>
     <row r="2" ht="24" customHeight="1">
       <c r="A2" s="3" t="inlineStr">
@@ -1365,29 +1363,38 @@
       <c r="C102" s="5" t="n"/>
     </row>
     <row r="103" ht="24" customHeight="1">
-      <c r="A103" s="3" t="inlineStr">
+      <c r="A103" s="4" t="inlineStr">
+        <is>
+          <t>Is there any backup equipment on site?</t>
+        </is>
+      </c>
+      <c r="B103" s="5" t="n"/>
+      <c r="C103" s="5" t="n"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="3" t="inlineStr">
         <is>
           <t>Documentation &amp; Handoff</t>
         </is>
       </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="4" t="inlineStr">
-        <is>
-          <t>Is there existing IT documentation? What platform (IT Glue, Passportal, wiki)?</t>
-        </is>
-      </c>
-      <c r="B104" s="5" t="n"/>
-      <c r="C104" s="5" t="n"/>
     </row>
     <row r="105">
       <c r="A105" s="4" t="inlineStr">
         <is>
-          <t>What admin credentials and accounts need to be transferred?</t>
+          <t>Is there existing IT documentation? What platform (IT Glue, Passportal, wiki)?</t>
         </is>
       </c>
       <c r="B105" s="5" t="n"/>
       <c r="C105" s="5" t="n"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="4" t="inlineStr">
+        <is>
+          <t>What admin credentials and accounts need to be transferred?</t>
+        </is>
+      </c>
+      <c r="B106" s="5" t="n"/>
+      <c r="C106" s="5" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>

<commit_message>
Fix merged cell conflict in Excel template for backup equipment row
Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/templates/rfi_template.xlsx
+++ b/templates/rfi_template.xlsx
@@ -57,7 +57,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -70,6 +70,34 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -455,7 +483,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C106"/>
+  <dimension ref="A1:C107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1368,8 +1396,6 @@
           <t>Is there any backup equipment on site?</t>
         </is>
       </c>
-      <c r="B103" s="5" t="n"/>
-      <c r="C103" s="5" t="n"/>
     </row>
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
@@ -1396,6 +1422,7 @@
       <c r="B106" s="5" t="n"/>
       <c r="C106" s="5" t="n"/>
     </row>
+    <row r="107"/>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A99:C99"/>
@@ -1405,12 +1432,12 @@
     <mergeCell ref="A85:C85"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A103:C103"/>
     <mergeCell ref="A54:C54"/>
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A104:C104"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Pre-refactor: speed optimizations, JSON repair, prompt improvements, field updates
- Extraction: 2 workers, smallest-first sorting, JSON repair fallback, per-job error isolation
- Prompt: distinguish prospect's current state from MSP's recommendations
- Schema: updated incumbent provider question, removed MSP cooperation & transition questions
- ReviewPage: fixed backup equipment category mapping (row 103)
- Template: updated row 20 question, blanked removed rows

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/templates/rfi_template.xlsx
+++ b/templates/rfi_template.xlsx
@@ -483,7 +483,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C107"/>
+  <dimension ref="A1:C106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -662,18 +662,14 @@
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
         <is>
-          <t>What is the current support type, quantity, and cadence?</t>
+          <t>Who is the incumbent provider and what is the current scope of services?</t>
         </is>
       </c>
       <c r="B20" s="5" t="n"/>
       <c r="C20" s="5" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="4" t="inlineStr">
-        <is>
-          <t>Is the outgoing MSP cooperative with the transition?</t>
-        </is>
-      </c>
+      <c r="A21" s="4" t="n"/>
       <c r="B21" s="5" t="n"/>
       <c r="C21" s="5" t="n"/>
     </row>
@@ -1422,7 +1418,6 @@
       <c r="B106" s="5" t="n"/>
       <c r="C106" s="5" t="n"/>
     </row>
-    <row r="107"/>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A99:C99"/>

</xml_diff>